<commit_message>
all solutions and metadata tables
</commit_message>
<xml_diff>
--- a/CAPS/CAPS Project Solutions/MetaData Tables/Bus Make.xlsx
+++ b/CAPS/CAPS Project Solutions/MetaData Tables/Bus Make.xlsx
@@ -36,14 +36,7 @@
     <x:xf numFmtId="22" applyNumberFormat="1"/>
     <x:xf numFmtId="49"/>
     <x:xf numFmtId="49"/>
-    <x:xf numFmtId="49"/>
-    <x:xf numFmtId="49"/>
-    <x:xf numFmtId="22" applyNumberFormat="1"/>
-    <x:xf numFmtId="49"/>
-    <x:xf numFmtId="49"/>
-    <x:xf numFmtId="22" applyNumberFormat="1"/>
     <x:xf numFmtId="0"/>
-    <x:xf numFmtId="14" applyNumberFormat="1"/>
     <x:xf numFmtId="49"/>
     <x:xf numFmtId="49"/>
   </x:cellXfs>
@@ -51,24 +44,17 @@
 </file>
 
 <file path=xl/tables/table.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O10" totalsRowShown="0">
-  <x:autoFilter ref="A1:O10"/>
-  <x:tableColumns count="15">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H10" totalsRowShown="0">
+  <x:autoFilter ref="A1:H10"/>
+  <x:tableColumns count="8">
     <x:tableColumn id="1" name="(Do Not Modify) Bus Make"/>
     <x:tableColumn id="2" name="(Do Not Modify) Row Checksum"/>
     <x:tableColumn id="3" name="(Do Not Modify) Modified On"/>
     <x:tableColumn id="4" name="Make"/>
     <x:tableColumn id="5" name="Manufacturer"/>
-    <x:tableColumn id="6" name="Created By"/>
-    <x:tableColumn id="7" name="Created By (Delegate)"/>
-    <x:tableColumn id="8" name="Created On"/>
-    <x:tableColumn id="9" name="Modified By"/>
-    <x:tableColumn id="10" name="Modified By (Delegate)"/>
-    <x:tableColumn id="11" name="Modified On"/>
-    <x:tableColumn id="12" name="Owner"/>
-    <x:tableColumn id="13" name="Record Created On"/>
-    <x:tableColumn id="14" name="Status"/>
-    <x:tableColumn id="15" name="Status Reason"/>
+    <x:tableColumn id="6" name="Owner"/>
+    <x:tableColumn id="7" name="Status"/>
+    <x:tableColumn id="8" name="Status Reason"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -80,7 +66,7 @@
   <x:sheetData>
     <x:row>
       <x:c r="A1" t="str">
-        <x:v>caps_busmake:xiTbNW1nyctAEch2fuJKdjJIQTGXepgbZs30DqooReEqKl/iLyLRQcqnAEnYTcSRqywogom8aFbht900jDZLyw==:caps_busmakeid=%28Do%20Not%20Modify%29%20Bus%20Make&amp;checksumLogicalName=%28Do%20Not%20Modify%29%20Row%20Checksum&amp;modifiedon=%28Do%20Not%20Modify%29%20Modified%20On&amp;caps_make=Make&amp;caps_manufacturer=Manufacturer&amp;createdby=Created%20By&amp;createdonbehalfby=Created%20By%20%28Delegate%29&amp;createdon=Created%20On&amp;modifiedby=Modified%20By&amp;modifiedonbehalfby=Modified%20By%20%28Delegate%29&amp;modifiedon=Modified%20On&amp;ownerid=Owner&amp;overriddencreatedon=Record%20Created%20On&amp;statecode=Status&amp;statuscode=Status%20Reason</x:v>
+        <x:v>caps_busmake:68ZahyIuysW596uTLzMRNOTy6f/AsxLqoG9Za/Xml8Z0w+urTXyc3tXG5w5zL9vVXo+vOspfPA7qjU5vQtH7Hg==:caps_busmakeid=%28Do%20Not%20Modify%29%20Bus%20Make&amp;checksumLogicalName=%28Do%20Not%20Modify%29%20Row%20Checksum&amp;modifiedon=%28Do%20Not%20Modify%29%20Modified%20On&amp;caps_make=Make&amp;caps_manufacturer=Manufacturer&amp;ownerid=Owner&amp;statecode=Status&amp;statuscode=Status%20Reason</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -106,7 +92,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="dataSheet"/>
-  <x:dimension ref="A1:O10"/>
+  <x:dimension ref="A1:H10"/>
   <x:sheetViews>
     <x:sheetView rightToLeft="0" tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -119,13 +105,6 @@
     <x:col min="6" max="6" width="14" style="6" hidden="0" customWidth="1"/>
     <x:col min="7" max="7" width="14" style="7" hidden="0" customWidth="1"/>
     <x:col min="8" max="8" width="14" style="8" hidden="0" customWidth="1"/>
-    <x:col min="9" max="9" width="14" style="9" hidden="0" customWidth="1"/>
-    <x:col min="10" max="10" width="14" style="10" hidden="0" customWidth="1"/>
-    <x:col min="11" max="11" width="14" style="11" hidden="0" customWidth="1"/>
-    <x:col min="12" max="12" width="14" style="12" hidden="0" customWidth="1"/>
-    <x:col min="13" max="13" width="14" style="13" hidden="0" customWidth="1"/>
-    <x:col min="14" max="14" width="14" style="14" hidden="0" customWidth="1"/>
-    <x:col min="15" max="15" width="14" style="15" hidden="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" hidden="0">
@@ -156,50 +135,15 @@
       </x:c>
       <x:c r="F1" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Created By</x:t>
+          <x:t xml:space="preserve">Owner</x:t>
         </x:is>
       </x:c>
       <x:c r="G1" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Created By (Delegate)</x:t>
+          <x:t xml:space="preserve">Status</x:t>
         </x:is>
       </x:c>
       <x:c r="H1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Created On</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="I1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Modified By</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Modified By (Delegate)</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="K1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Modified On</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="L1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Owner</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Record Created On</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="N1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Status</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O1" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Status Reason</x:t>
         </x:is>
@@ -213,7 +157,7 @@
       </x:c>
       <x:c r="B2" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">DAhG5gleaUPCVmJuXXjFvqhEoBV4lE6oCCU8qaXnCLGRuGFVIDbSSVh4pz9ak2l7KI1NKQiIE6tiNDWQRM77Vw==</x:t>
+          <x:t xml:space="preserve">uYsjwhSYS6T2y7ph58Ih+GaD1P610n5jb4CHcoNwhwm0iUb7kir+OV1+Z7FOpsDC1rxqH0MPBoZMD3RhXO/5zA==</x:t>
         </x:is>
       </x:c>
       <x:c r="C2" s="3">
@@ -234,31 +178,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G2" s="7"/>
-      <x:c r="H2" s="8">
-        <x:v>43937.4787037037</x:v>
-      </x:c>
-      <x:c r="I2" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J2" s="10"/>
-      <x:c r="K2" s="11">
-        <x:v>43937.4787037037</x:v>
-      </x:c>
-      <x:c r="L2" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M2" s="13"/>
-      <x:c r="N2" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O2" s="15" t="inlineStr">
+      <x:c r="G2" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H2" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -272,7 +197,7 @@
       </x:c>
       <x:c r="B3" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">iqhmvlH3X9hz9TfwQGeVOiNl5L26qe63KI+OC09jDMdHTtuJRm39zzRxvHQGaOSoe1hIazNtFeOGxanKBupgNg==</x:t>
+          <x:t xml:space="preserve">Q2HhobEpGmPbG+K1MIlewUSVz7BHLmK0bpEMKAx5AZMbirAJvRN67Z8oXcUuyofZb+ax29gJvokUZdnBmyKebA==</x:t>
         </x:is>
       </x:c>
       <x:c r="C3" s="3">
@@ -293,31 +218,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G3" s="7"/>
-      <x:c r="H3" s="8">
-        <x:v>43937.4798263889</x:v>
-      </x:c>
-      <x:c r="I3" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J3" s="10"/>
-      <x:c r="K3" s="11">
-        <x:v>43956.5987615741</x:v>
-      </x:c>
-      <x:c r="L3" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M3" s="13"/>
-      <x:c r="N3" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O3" s="15" t="inlineStr">
+      <x:c r="G3" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H3" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -331,7 +237,7 @@
       </x:c>
       <x:c r="B4" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">ymhMVv46cTfGG4/Lxk9IpvsWb7nOZwvusIAAywU+hJ3SW7ibuN6hfnb5OeDW++8FtwQttuYjF9aF38foBSp7Yg==</x:t>
+          <x:t xml:space="preserve">30FAUX5R/BsxtvZlum6+lLfArOn6UF0MKF+kOTIBSseGI7ncZBy/21t8+3WJpT78WvKmoT5pT3zbVszs2ediDA==</x:t>
         </x:is>
       </x:c>
       <x:c r="C4" s="3">
@@ -352,31 +258,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G4" s="7"/>
-      <x:c r="H4" s="8">
-        <x:v>43937.4808217593</x:v>
-      </x:c>
-      <x:c r="I4" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J4" s="10"/>
-      <x:c r="K4" s="11">
-        <x:v>43937.4808217593</x:v>
-      </x:c>
-      <x:c r="L4" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M4" s="13"/>
-      <x:c r="N4" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O4" s="15" t="inlineStr">
+      <x:c r="G4" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H4" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -390,7 +277,7 @@
       </x:c>
       <x:c r="B5" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">LygS7RmdvMyL2T4/awY1ge2KAcR7XYpIyw4F1AvmkhjmmA74MjrNk5dUwvF8wHDRDqHx6qKjqr6mzSvYBNJlXw==</x:t>
+          <x:t xml:space="preserve">d61TRg+bHfWq27Tf0z73f2Fv4ApyBfBxMRhecq2cfVnkkVjnVfHWJKv06cFQhu+KZa03qtxOxHIeIfpJBxWa9Q==</x:t>
         </x:is>
       </x:c>
       <x:c r="C5" s="3">
@@ -411,31 +298,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G5" s="7"/>
-      <x:c r="H5" s="8">
-        <x:v>43937.4805324074</x:v>
-      </x:c>
-      <x:c r="I5" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J5" s="10"/>
-      <x:c r="K5" s="11">
-        <x:v>43937.4805324074</x:v>
-      </x:c>
-      <x:c r="L5" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M5" s="13"/>
-      <x:c r="N5" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O5" s="15" t="inlineStr">
+      <x:c r="G5" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H5" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -449,7 +317,7 @@
       </x:c>
       <x:c r="B6" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">dhw92ecrVZGjDy30P6b84hww1zPmgLMsIoSbputc1ZtRmFZ6FrwFKoReT2DtPakTUl/b9wUXXjszu8IW/ZXyFQ==</x:t>
+          <x:t xml:space="preserve">eyb4nTOG7m0kuF5EhDyTT/a6Ck4bwFOtfMAKxoq4auZK22K5LBoyBI6kku8sF06uHLGjCC6uDJL1b5c6ZtNGBQ==</x:t>
         </x:is>
       </x:c>
       <x:c r="C6" s="3">
@@ -470,31 +338,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G6" s="7"/>
-      <x:c r="H6" s="8">
-        <x:v>43937.4802893518</x:v>
-      </x:c>
-      <x:c r="I6" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J6" s="10"/>
-      <x:c r="K6" s="11">
-        <x:v>43937.4802893518</x:v>
-      </x:c>
-      <x:c r="L6" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M6" s="13"/>
-      <x:c r="N6" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O6" s="15" t="inlineStr">
+      <x:c r="G6" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H6" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -508,7 +357,7 @@
       </x:c>
       <x:c r="B7" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">4DQD9NeW/gZKHRAjEaHyzQzUKdwbsyzQovpAGykV2JBI39T4GwAoxEU4Rxmg/ugeo61cYE4nyII0tiBJMApHfg==</x:t>
+          <x:t xml:space="preserve">dmNfgpK3L/GK1gUwJsDTRxla7w3oc/VzyRjqZruU+LeG2ymFDtuv7mwv9VkafEwOzB9l+tQKfgOaQ2oGqvX8hA==</x:t>
         </x:is>
       </x:c>
       <x:c r="C7" s="3">
@@ -529,31 +378,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G7" s="7"/>
-      <x:c r="H7" s="8">
-        <x:v>43937.4793287037</x:v>
-      </x:c>
-      <x:c r="I7" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J7" s="10"/>
-      <x:c r="K7" s="11">
-        <x:v>43937.4793287037</x:v>
-      </x:c>
-      <x:c r="L7" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M7" s="13"/>
-      <x:c r="N7" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O7" s="15" t="inlineStr">
+      <x:c r="G7" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H7" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -567,7 +397,7 @@
       </x:c>
       <x:c r="B8" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">ZL+Y7aYKf1+CJdieS+xcB9FE1LQ6orbGR/SfPi28oFzg58jDXzoaHvTgXHhIPufsyl5xl/1lJ+m3KErcmjefgQ==</x:t>
+          <x:t xml:space="preserve">tJzUpaZ6q5NQXxxKqlfEXdRN7jeXR6nyL/pxy3BMSFV4EnK3bJzVyeKZel5v9OOPbrmd8VXPTOGS6/usP/d5vw==</x:t>
         </x:is>
       </x:c>
       <x:c r="C8" s="3">
@@ -588,31 +418,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G8" s="7"/>
-      <x:c r="H8" s="8">
-        <x:v>43937.4791898148</x:v>
-      </x:c>
-      <x:c r="I8" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J8" s="10"/>
-      <x:c r="K8" s="11">
-        <x:v>43937.4791898148</x:v>
-      </x:c>
-      <x:c r="L8" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M8" s="13"/>
-      <x:c r="N8" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O8" s="15" t="inlineStr">
+      <x:c r="G8" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H8" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -626,7 +437,7 @@
       </x:c>
       <x:c r="B9" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">hIxA5sqEg3j8mmQ8QX/91fnqQMS+Q/mjTlpqkSnDb0L9Vpa6Xr5x9dlvZRYwwxL4ChiB2129LnGU73fxF9p0aQ==</x:t>
+          <x:t xml:space="preserve">irM6VRDWabQ+RpgxcFWvwLrvYAwik7mN9X8jebJ30gsMZqeg2r9S+hfKcgrvu9+UvTmuUNvGALyGAqrnRVr8xA==</x:t>
         </x:is>
       </x:c>
       <x:c r="C9" s="3">
@@ -647,31 +458,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G9" s="7"/>
-      <x:c r="H9" s="8">
-        <x:v>43937.4796412037</x:v>
-      </x:c>
-      <x:c r="I9" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J9" s="10"/>
-      <x:c r="K9" s="11">
-        <x:v>43937.4796412037</x:v>
-      </x:c>
-      <x:c r="L9" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M9" s="13"/>
-      <x:c r="N9" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O9" s="15" t="inlineStr">
+      <x:c r="G9" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H9" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -685,7 +477,7 @@
       </x:c>
       <x:c r="B10" s="2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">X75wEKU3KuWbBCq7jxg1A54gmtQTIQkOvK7kev2nPz4zhqBcy/EyRj10i+3gA7fP8O5ad1tkUHqtgAWck575Bw==</x:t>
+          <x:t xml:space="preserve">o1Mq5xQXrp2/2K8dhACjpPiV/OJl5N1GwlwxnZ5rmRkyQjnE2V+x1spAox+mOzsRQSsJjyAK1ekFvO212IQsPQ==</x:t>
         </x:is>
       </x:c>
       <x:c r="C10" s="3">
@@ -706,31 +498,12 @@
           <x:t xml:space="preserve">Albus Dumbledore</x:t>
         </x:is>
       </x:c>
-      <x:c r="G10" s="7"/>
-      <x:c r="H10" s="8">
-        <x:v>43937.4789930556</x:v>
-      </x:c>
-      <x:c r="I10" s="9" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="J10" s="10"/>
-      <x:c r="K10" s="11">
-        <x:v>43937.4789930556</x:v>
-      </x:c>
-      <x:c r="L10" s="12" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Albus Dumbledore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="M10" s="13"/>
-      <x:c r="N10" s="14" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Active</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="O10" s="15" t="inlineStr">
+      <x:c r="G10" s="7" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Active</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="H10" s="8" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Active</x:t>
         </x:is>
@@ -747,24 +520,11 @@
     <x:dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="0" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 100 characters long." promptTitle="Text (required)" prompt="Maximum Length: 100 characters." sqref="E2:E1048576">
       <x:formula1>100</x:formula1>
     </x:dataValidation>
-    <x:dataValidation type="none" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="" error=" " promptTitle="Lookup" prompt="This Created By record must already exist in Microsoft Dynamics 365 or in this source file." sqref="F2:F1048576"/>
-    <x:dataValidation type="none" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="" error=" " promptTitle="Lookup" prompt="This Created By (Delegate) record must already exist in Microsoft Dynamics 365 or in this source file." sqref="G2:G1048576"/>
-    <x:dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="Created On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="H2:H1048576">
-      <x:formula1>1</x:formula1>
-    </x:dataValidation>
-    <x:dataValidation type="none" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="" error=" " promptTitle="Lookup" prompt="This Modified By record must already exist in Microsoft Dynamics 365 or in this source file." sqref="I2:I1048576"/>
-    <x:dataValidation type="none" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="" error=" " promptTitle="Lookup" prompt="This Modified By (Delegate) record must already exist in Microsoft Dynamics 365 or in this source file." sqref="J2:J1048576"/>
-    <x:dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="Modified On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="K2:K1048576">
-      <x:formula1>1</x:formula1>
-    </x:dataValidation>
-    <x:dataValidation type="none" allowBlank="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics 365 or in this source file." sqref="L2:L1048576"/>
-    <x:dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="Record Created On must be in the correct date format." promptTitle="Date" prompt=" " sqref="M2:M1048576">
-      <x:formula1>1</x:formula1>
-    </x:dataValidation>
-    <x:dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="Status must be selected from the drop-down list." promptTitle="Option set (required)" prompt="Select a value from the drop-down list." sqref="N2:N1048576">
+    <x:dataValidation type="none" allowBlank="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics 365 or in this source file." sqref="F2:F1048576"/>
+    <x:dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="Status must be selected from the drop-down list." promptTitle="Option set (required)" prompt="Select a value from the drop-down list." sqref="G2:G1048576">
       <x:formula1>hiddenSheet!$A$2:$B$2</x:formula1>
     </x:dataValidation>
-    <x:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="Status Reason must be selected from the drop-down list." promptTitle="Option set" prompt="Select a value from the drop-down list." sqref="O2:O1048576">
+    <x:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="Status Reason must be selected from the drop-down list." promptTitle="Option set" prompt="Select a value from the drop-down list." sqref="H2:H1048576">
       <x:formula1>hiddenSheet!$A$3:$B$3</x:formula1>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>